<commit_message>
Sisia produccion falta con muchos
</commit_message>
<xml_diff>
--- a/Documentacion/respaldo_ok.xlsx
+++ b/Documentacion/respaldo_ok.xlsx
@@ -4484,7 +4484,7 @@
     <t>Demo de las estrategias_152</t>
   </si>
   <si>
-    <t>RACG770826MBCMSS</t>
+    <t>PECJ971112HMCRHN</t>
   </si>
 </sst>
 </file>
@@ -12411,8 +12411,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:AU160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F120" workbookViewId="0">
-      <selection activeCell="P146" sqref="P146:P147"/>
+    <sheetView tabSelected="1" topLeftCell="D108" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12471,7 +12471,7 @@
         <v>1</v>
       </c>
       <c r="M1">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="N1">
         <v>5540657801</v>
@@ -12564,7 +12564,7 @@
         <v>2</v>
       </c>
       <c r="AR1" s="56">
-        <v>256850</v>
+        <v>234.34</v>
       </c>
       <c r="AS1" s="58" t="s">
         <v>1331</v>
@@ -12703,7 +12703,7 @@
         <v>4</v>
       </c>
       <c r="AR2" s="56">
-        <v>125820</v>
+        <v>3456.56</v>
       </c>
       <c r="AS2" s="58" t="s">
         <v>1332</v>
@@ -32577,6 +32577,7 @@
     </row>
     <row r="148" spans="1:47" x14ac:dyDescent="0.3">
       <c r="L148" s="50"/>
+      <c r="P148" s="61"/>
       <c r="W148" s="51"/>
       <c r="X148" s="51"/>
       <c r="AP148" s="54"/>
@@ -32585,6 +32586,7 @@
     </row>
     <row r="149" spans="1:47" x14ac:dyDescent="0.3">
       <c r="L149" s="50"/>
+      <c r="P149" s="61"/>
       <c r="W149" s="51"/>
       <c r="X149" s="51"/>
       <c r="Y149" s="51"/>
@@ -32594,6 +32596,7 @@
     </row>
     <row r="150" spans="1:47" x14ac:dyDescent="0.3">
       <c r="L150" s="50"/>
+      <c r="P150" s="61"/>
       <c r="W150" s="51"/>
       <c r="X150" s="51"/>
       <c r="Y150" s="51"/>
@@ -32603,6 +32606,7 @@
     </row>
     <row r="151" spans="1:47" x14ac:dyDescent="0.3">
       <c r="L151" s="50"/>
+      <c r="P151" s="61"/>
       <c r="W151" s="51"/>
       <c r="X151" s="51"/>
       <c r="Y151" s="51"/>
@@ -32612,6 +32616,7 @@
     </row>
     <row r="152" spans="1:47" x14ac:dyDescent="0.3">
       <c r="L152" s="50"/>
+      <c r="P152" s="61"/>
       <c r="W152" s="51"/>
       <c r="X152" s="51"/>
       <c r="Y152" s="51"/>

</xml_diff>

<commit_message>
Cambios de botones y campos id todo ok
</commit_message>
<xml_diff>
--- a/Documentacion/respaldo_ok.xlsx
+++ b/Documentacion/respaldo_ok.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6128" uniqueCount="1485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6128" uniqueCount="1486">
   <si>
     <t>id_usuario</t>
   </si>
@@ -4485,6 +4485,9 @@
   </si>
   <si>
     <t>PECJ971112HMCRHN</t>
+  </si>
+  <si>
+    <t>AUSJ8302134T</t>
   </si>
 </sst>
 </file>
@@ -12412,7 +12415,7 @@
   <dimension ref="A1:AU160"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D108" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P145"/>
+      <selection activeCell="O108" sqref="O108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27323,7 +27326,7 @@
         <v>5540657894</v>
       </c>
       <c r="O108" t="s">
-        <v>1292</v>
+        <v>1485</v>
       </c>
       <c r="P108" s="61" t="s">
         <v>1484</v>

</xml_diff>